<commit_message>
update orgUnit tranlsation using json format
</commit_message>
<xml_diff>
--- a/sample-format/dataElementsUpdate.xlsx
+++ b/sample-format/dataElementsUpdate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mithilesh Thakur\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EAF63C-EC8A-4B86-960A-CDA26E8DD7F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76395177-502D-4D48-8164-016B886FD123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="1917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="1919">
   <si>
     <t>name</t>
   </si>
@@ -5810,6 +5810,12 @@
   </si>
   <si>
     <t>Insufficient ace water allyear round(Not improved)</t>
+  </si>
+  <si>
+    <t>aggregationType</t>
+  </si>
+  <si>
+    <t>LAST</t>
   </si>
 </sst>
 </file>
@@ -6180,10 +6186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6B5FAB-DF4A-42DC-8643-A674828EC12D}">
-  <dimension ref="A1:E416"/>
+  <dimension ref="A1:F416"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6192,9 +6198,11 @@
     <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.08984375" customWidth="1"/>
+    <col min="5" max="5" width="33.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1907</v>
       </c>
@@ -6210,8 +6218,11 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -6227,8 +6238,11 @@
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -6244,8 +6258,11 @@
       <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -6262,7 +6279,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -6279,7 +6296,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -6296,7 +6313,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -6313,7 +6330,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
@@ -6330,7 +6347,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
@@ -6347,7 +6364,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>44</v>
       </c>
@@ -6364,7 +6381,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>49</v>
       </c>
@@ -6381,7 +6398,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>54</v>
       </c>
@@ -6398,7 +6415,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>59</v>
       </c>
@@ -6415,7 +6432,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>64</v>
       </c>
@@ -6432,7 +6449,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>69</v>
       </c>
@@ -6449,7 +6466,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>74</v>
       </c>
@@ -13273,12 +13290,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064994C001712374395B345EB88ED991F" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c1a62579524e26006c6d5335831b55c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f9770305-a86c-4dd4-a8e3-5283c3e6bf99" xmlns:ns3="3f48127a-ff27-4c8f-88c3-e54b29f41588" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="658091719f3253a39288b5ed2add5a7b" ns2:_="" ns3:_="">
     <xsd:import namespace="f9770305-a86c-4dd4-a8e3-5283c3e6bf99"/>
@@ -13475,6 +13486,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -13485,15 +13502,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E76993AC-6818-4630-B1D6-F654BE5E03B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13512,6 +13520,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
   <ds:schemaRefs>

</xml_diff>